<commit_message>
add instructors to newsubject xslx
</commit_message>
<xml_diff>
--- a/Timetable-template.xlsx
+++ b/Timetable-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ducle/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ducle/Desktop/unitime-do-an/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{934DB122-90C8-3747-8FD4-F89959902EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF76FE5-3FAE-BD40-8684-ADD6E1F81B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="54560" yWindow="5300" windowWidth="22560" windowHeight="21260" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10280" yWindow="10820" windowWidth="31800" windowHeight="22020" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Subject" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="76">
   <si>
     <t>NUM_LAB_HOURS</t>
   </si>
@@ -256,6 +256,9 @@
   </si>
   <si>
     <t>CLASS_TYPE</t>
+  </si>
+  <si>
+    <t>INSTRUCTORS</t>
   </si>
 </sst>
 </file>
@@ -1065,7 +1068,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -2321,10 +2324,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2336,7 +2339,7 @@
     <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2361,8 +2364,11 @@
       <c r="H1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -2387,8 +2393,11 @@
       <c r="H2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -2413,8 +2422,11 @@
       <c r="H3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -2439,8 +2451,11 @@
       <c r="H4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2465,8 +2480,11 @@
       <c r="H5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -2491,8 +2509,11 @@
       <c r="H6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -2514,8 +2535,11 @@
       <c r="G7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -2540,8 +2564,11 @@
       <c r="H8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -2562,6 +2589,9 @@
       </c>
       <c r="G9">
         <v>2</v>
+      </c>
+      <c r="I9">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update excel template & adapter
</commit_message>
<xml_diff>
--- a/Timetable-template.xlsx
+++ b/Timetable-template.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ducle/Desktop/unitime-do-an/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs\BK - HCMUT\Programs\Github\unitime-do-an\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF76FE5-3FAE-BD40-8684-ADD6E1F81B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10280" yWindow="10820" windowWidth="31800" windowHeight="22020" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10275" yWindow="10815" windowWidth="31800" windowHeight="22020" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Subject" sheetId="1" r:id="rId1"/>
@@ -19,7 +18,6 @@
     <sheet name="Student" sheetId="9" r:id="rId4"/>
     <sheet name="Enrollment" sheetId="10" r:id="rId5"/>
     <sheet name="Class" sheetId="7" r:id="rId6"/>
-    <sheet name="NewSubject" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="81">
   <si>
     <t>NUM_LAB_HOURS</t>
   </si>
@@ -255,16 +253,31 @@
     <t>STUDENT_ID</t>
   </si>
   <si>
-    <t>CLASS_TYPE</t>
-  </si>
-  <si>
     <t>INSTRUCTORS</t>
+  </si>
+  <si>
+    <t>0,1</t>
+  </si>
+  <si>
+    <t>3,4</t>
+  </si>
+  <si>
+    <t>5,6</t>
+  </si>
+  <si>
+    <t>LAB_TYPE</t>
+  </si>
+  <si>
+    <t>LEC_CAPACITY</t>
+  </si>
+  <si>
+    <t>LAB_CAPACITY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -609,117 +622,269 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" customWidth="1"/>
+    <col min="1" max="1" width="14.125" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="15.625" customWidth="1"/>
+    <col min="5" max="5" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2">
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="J4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="J5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="J6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="J7">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="J8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="J9">
         <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -728,21 +893,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.375" customWidth="1"/>
     <col min="7" max="8" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -759,7 +924,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -773,7 +938,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -787,7 +952,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -801,7 +966,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -818,7 +983,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -835,7 +1000,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -852,7 +1017,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -866,7 +1031,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -883,7 +1048,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -897,7 +1062,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -914,7 +1079,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -937,19 +1102,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -960,7 +1125,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -971,7 +1136,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -982,7 +1147,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -993,7 +1158,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1004,7 +1169,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1015,7 +1180,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1026,7 +1191,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1037,7 +1202,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1048,7 +1213,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1065,19 +1230,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1088,7 +1253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1099,7 +1264,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1110,7 +1275,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1121,7 +1286,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1132,7 +1297,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1143,7 +1308,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1154,7 +1319,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1165,7 +1330,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1176,7 +1341,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1187,7 +1352,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1198,7 +1363,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1209,7 +1374,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1220,7 +1385,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1231,7 +1396,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1242,7 +1407,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1259,20 +1424,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:C58"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1280,10 +1446,13 @@
         <v>72</v>
       </c>
       <c r="C1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1293,8 +1462,11 @@
       <c r="C2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1302,10 +1474,13 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1313,10 +1488,13 @@
         <v>0</v>
       </c>
       <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1324,10 +1502,13 @@
         <v>0</v>
       </c>
       <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1335,10 +1516,13 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1346,10 +1530,13 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1357,10 +1544,13 @@
         <v>1</v>
       </c>
       <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1368,10 +1558,13 @@
         <v>1</v>
       </c>
       <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1379,10 +1572,13 @@
         <v>2</v>
       </c>
       <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1390,10 +1586,13 @@
         <v>2</v>
       </c>
       <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1401,10 +1600,13 @@
         <v>2</v>
       </c>
       <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1412,10 +1614,13 @@
         <v>2</v>
       </c>
       <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1423,10 +1628,13 @@
         <v>3</v>
       </c>
       <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1434,10 +1642,13 @@
         <v>3</v>
       </c>
       <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1445,10 +1656,13 @@
         <v>3</v>
       </c>
       <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1458,8 +1672,11 @@
       <c r="C17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1467,10 +1684,13 @@
         <v>4</v>
       </c>
       <c r="C18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1478,10 +1698,13 @@
         <v>4</v>
       </c>
       <c r="C19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1489,10 +1712,13 @@
         <v>5</v>
       </c>
       <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1500,10 +1726,13 @@
         <v>5</v>
       </c>
       <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1511,295 +1740,406 @@
         <v>5</v>
       </c>
       <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26">
         <v>7</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27">
         <v>7</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28">
         <v>7</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29">
         <v>8</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="B30">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
       <c r="B31">
         <v>8</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
       <c r="B32">
         <v>9</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
       <c r="B33">
         <v>9</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
       <c r="B34">
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
       <c r="B35">
         <v>10</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
       <c r="B36">
         <v>10</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
       <c r="B37">
         <v>10</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
       <c r="B38">
         <v>11</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
       <c r="B39">
         <v>11</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
       <c r="B40">
         <v>11</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
       <c r="B41">
         <v>12</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C41">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
       <c r="B42">
         <v>12</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C42">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
       <c r="B43">
         <v>12</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
       <c r="B44">
         <v>13</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C44">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
       <c r="B45">
         <v>13</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
       <c r="B46">
         <v>13</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C46">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
       <c r="B47">
         <v>14</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C47">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
       <c r="B48">
         <v>14</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C48">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
       <c r="B49">
         <v>14</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C49">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
       <c r="B50">
         <v>15</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C50">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
       <c r="B51">
         <v>15</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C51">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>50</v>
       </c>
       <c r="B52">
         <v>15</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C52">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>51</v>
       </c>
       <c r="B53">
         <v>16</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C53">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>52</v>
       </c>
       <c r="B54">
         <v>16</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C54">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>53</v>
       </c>
       <c r="B55">
         <v>16</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C55">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>54</v>
       </c>
       <c r="B56">
         <v>17</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C56">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>55</v>
       </c>
       <c r="B57">
         <v>17</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C57">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>56</v>
       </c>
       <c r="B58">
         <v>17</v>
+      </c>
+      <c r="C58">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1808,22 +2148,22 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1849,7 +2189,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1875,7 +2215,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1901,7 +2241,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1927,7 +2267,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1953,7 +2293,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1979,7 +2319,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2005,7 +2345,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2031,7 +2371,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2057,7 +2397,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2083,7 +2423,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2109,7 +2449,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2135,7 +2475,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2161,7 +2501,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2187,7 +2527,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2213,7 +2553,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2239,7 +2579,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2265,7 +2605,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2291,7 +2631,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2315,283 +2655,6 @@
       </c>
       <c r="H19">
         <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:I9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="14.1640625" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2">
-        <v>4</v>
-      </c>
-      <c r="H2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3">
-        <v>3</v>
-      </c>
-      <c r="H3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4">
-        <v>2</v>
-      </c>
-      <c r="H4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I4">
-        <v>3.4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5">
-        <v>2</v>
-      </c>
-      <c r="H5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5">
-        <v>3.4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6">
-        <v>2</v>
-      </c>
-      <c r="H6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I6">
-        <v>5.6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7">
-        <v>2</v>
-      </c>
-      <c r="I7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8">
-        <v>2</v>
-      </c>
-      <c r="H8" t="s">
-        <v>3</v>
-      </c>
-      <c r="I8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>2</v>
-      </c>
-      <c r="E9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9">
-        <v>2</v>
-      </c>
-      <c r="I9">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update excel template example
</commit_message>
<xml_diff>
--- a/Timetable-template.xlsx
+++ b/Timetable-template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10275" yWindow="10815" windowWidth="31800" windowHeight="22020" activeTab="5"/>
+    <workbookView xWindow="10275" yWindow="10815" windowWidth="31800" windowHeight="22020"/>
   </bookViews>
   <sheets>
     <sheet name="Subject" sheetId="1" r:id="rId1"/>
@@ -625,15 +625,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.125" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="15.625" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
@@ -649,10 +649,10 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E1" t="s">
         <v>13</v>
@@ -681,10 +681,10 @@
         <v>11</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E2" t="s">
         <v>19</v>
@@ -713,10 +713,10 @@
         <v>12</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E3" t="s">
         <v>19</v>
@@ -739,10 +739,10 @@
         <v>16</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E4" t="s">
         <v>19</v>
@@ -765,10 +765,10 @@
         <v>18</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E5" t="s">
         <v>19</v>
@@ -791,10 +791,10 @@
         <v>20</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>
@@ -817,10 +817,10 @@
         <v>25</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E7" t="s">
         <v>19</v>
@@ -843,10 +843,10 @@
         <v>23</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E8" t="s">
         <v>19</v>
@@ -869,10 +869,10 @@
         <v>24</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E9" t="s">
         <v>19</v>
@@ -1425,10 +1425,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1756,6 +1756,9 @@
       <c r="C23">
         <v>2</v>
       </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
@@ -1767,6 +1770,9 @@
       <c r="C24">
         <v>2</v>
       </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
@@ -1778,6 +1784,9 @@
       <c r="C25">
         <v>2</v>
       </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
@@ -1789,6 +1798,9 @@
       <c r="C26">
         <v>2</v>
       </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
@@ -1800,16 +1812,22 @@
       <c r="C27">
         <v>2</v>
       </c>
+      <c r="D27">
+        <v>4</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="D28">
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1822,16 +1840,22 @@
       <c r="C29">
         <v>3</v>
       </c>
+      <c r="D29">
+        <v>4</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="B30">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C30">
         <v>3</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1839,10 +1863,13 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C31">
         <v>3</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1855,30 +1882,39 @@
       <c r="C32">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
       <c r="B33">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C33">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="D33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
       <c r="B34">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C34">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="D34">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
@@ -1888,258 +1924,345 @@
       <c r="C35">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
       <c r="B36">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C36">
         <v>4</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
       <c r="B37">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C37">
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
       <c r="B38">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C38">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="D38">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
       <c r="B39">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C39">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="D39">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
       <c r="B40">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C40">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="D40">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
       <c r="B41">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C41">
         <v>5</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
       <c r="B42">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C42">
         <v>5</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
       <c r="B43">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C43">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="D43">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
       <c r="B44">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C44">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="D44">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
       <c r="B45">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C45">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="D45">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
       <c r="B46">
+        <v>15</v>
+      </c>
+      <c r="C46">
+        <v>6</v>
+      </c>
+      <c r="D46">
         <v>13</v>
       </c>
-      <c r="C46">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
       <c r="B47">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C47">
         <v>6</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
       <c r="B48">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C48">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="D48">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
       <c r="B49">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C49">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="D49">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
       <c r="B50">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C50">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="D50">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
       <c r="B51">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C51">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="D51">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>50</v>
       </c>
       <c r="B52">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C52">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="D52">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>51</v>
       </c>
-      <c r="B53">
-        <v>16</v>
-      </c>
       <c r="C53">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>52</v>
       </c>
-      <c r="B54">
-        <v>16</v>
-      </c>
       <c r="C54">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>53</v>
       </c>
-      <c r="B55">
-        <v>16</v>
-      </c>
       <c r="C55">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>54</v>
       </c>
-      <c r="B56">
-        <v>17</v>
-      </c>
       <c r="C56">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>55</v>
       </c>
-      <c r="B57">
-        <v>17</v>
-      </c>
       <c r="C57">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>56</v>
       </c>
-      <c r="B58">
-        <v>17</v>
-      </c>
       <c r="C58">
-        <v>7</v>
+        <v>1</v>
+      </c>
+      <c r="D58">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>58</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+      <c r="D60">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>59</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -2151,8 +2274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
[xlsx] change import interface + raise engine bugs
</commit_message>
<xml_diff>
--- a/Timetable-template.xlsx
+++ b/Timetable-template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs\BK - HCMUT\Programs\Github\unitime-do-an\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ducle/Desktop/unitime-do-an/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9920D681-5E9A-694F-B0DE-D33539C0C165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10275" yWindow="10815" windowWidth="31800" windowHeight="22020"/>
+    <workbookView xWindow="1460" yWindow="1840" windowWidth="31800" windowHeight="22020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Subject" sheetId="1" r:id="rId1"/>
@@ -112,9 +113,6 @@
     <t>LABEL</t>
   </si>
   <si>
-    <t>TYPE</t>
-  </si>
-  <si>
     <t>H1-101</t>
   </si>
   <si>
@@ -272,16 +270,25 @@
   </si>
   <si>
     <t>LAB_CAPACITY</t>
+  </si>
+  <si>
+    <t>CLASS_TYPE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -622,26 +629,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.125" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -661,19 +669,19 @@
         <v>14</v>
       </c>
       <c r="G1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" t="s">
         <v>79</v>
       </c>
-      <c r="H1" t="s">
-        <v>80</v>
-      </c>
       <c r="I1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -702,10 +710,10 @@
         <v>3</v>
       </c>
       <c r="J2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -731,7 +739,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -754,10 +762,10 @@
         <v>2</v>
       </c>
       <c r="J4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -780,10 +788,10 @@
         <v>2</v>
       </c>
       <c r="J5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -806,10 +814,10 @@
         <v>2</v>
       </c>
       <c r="J6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -835,7 +843,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -861,7 +869,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -888,26 +896,27 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.375" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
     <col min="7" max="8" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -921,57 +930,57 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>28</v>
       </c>
-      <c r="D2">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>29</v>
       </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>30</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>31</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -983,12 +992,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
         <v>21</v>
@@ -1000,12 +1009,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
         <v>22</v>
@@ -1017,12 +1026,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8">
         <v>4</v>
@@ -1031,12 +1040,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -1048,12 +1057,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10">
         <v>3</v>
@@ -1062,12 +1071,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
         <v>21</v>
@@ -1079,12 +1088,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
         <v>22</v>
@@ -1102,19 +1111,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1125,7 +1134,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1133,10 +1142,10 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1144,10 +1153,10 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1155,10 +1164,10 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1166,10 +1175,10 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1177,10 +1186,10 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1188,10 +1197,10 @@
         <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1199,10 +1208,10 @@
         <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1210,10 +1219,10 @@
         <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1221,7 +1230,7 @@
         <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1230,19 +1239,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1253,166 +1262,166 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C16" t="s">
         <v>22</v>
@@ -1424,35 +1433,35 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" t="s">
         <v>72</v>
       </c>
-      <c r="C1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1466,7 +1475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1480,7 +1489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1494,7 +1503,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1508,7 +1517,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1522,7 +1531,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1536,7 +1545,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1550,7 +1559,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1564,7 +1573,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1578,7 +1587,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1592,7 +1601,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1606,7 +1615,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1620,7 +1629,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1634,7 +1643,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1648,7 +1657,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1662,7 +1671,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1676,7 +1685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1690,7 +1699,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1704,7 +1713,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1718,7 +1727,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1732,7 +1741,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1746,7 +1755,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1760,7 +1769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1774,7 +1783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1788,7 +1797,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1802,7 +1811,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1816,7 +1825,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1830,7 +1839,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1844,7 +1853,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1858,7 +1867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1872,7 +1881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1886,7 +1895,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1900,7 +1909,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>32</v>
       </c>
@@ -1914,7 +1923,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>33</v>
       </c>
@@ -1928,7 +1937,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>34</v>
       </c>
@@ -1942,7 +1951,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>35</v>
       </c>
@@ -1956,7 +1965,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>36</v>
       </c>
@@ -1970,7 +1979,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>37</v>
       </c>
@@ -1984,7 +1993,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>38</v>
       </c>
@@ -1998,7 +2007,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>39</v>
       </c>
@@ -2012,7 +2021,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>40</v>
       </c>
@@ -2026,7 +2035,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>41</v>
       </c>
@@ -2040,7 +2049,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>42</v>
       </c>
@@ -2054,7 +2063,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>43</v>
       </c>
@@ -2068,7 +2077,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>44</v>
       </c>
@@ -2082,7 +2091,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>45</v>
       </c>
@@ -2096,7 +2105,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>46</v>
       </c>
@@ -2110,7 +2119,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>47</v>
       </c>
@@ -2124,7 +2133,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>48</v>
       </c>
@@ -2138,7 +2147,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>49</v>
       </c>
@@ -2152,7 +2161,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>50</v>
       </c>
@@ -2166,7 +2175,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>51</v>
       </c>
@@ -2177,7 +2186,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>52</v>
       </c>
@@ -2188,7 +2197,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>53</v>
       </c>
@@ -2199,7 +2208,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>54</v>
       </c>
@@ -2210,7 +2219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>55</v>
       </c>
@@ -2221,7 +2230,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>56</v>
       </c>
@@ -2232,7 +2241,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>57</v>
       </c>
@@ -2243,7 +2252,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>58</v>
       </c>
@@ -2254,7 +2263,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>59</v>
       </c>
@@ -2271,48 +2280,48 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" t="s">
         <v>63</v>
       </c>
-      <c r="C1" t="s">
-        <v>64</v>
-      </c>
       <c r="D1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E1" t="s">
         <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" t="s">
         <v>68</v>
       </c>
-      <c r="H1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2326,7 +2335,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -2338,7 +2347,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2352,7 +2361,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -2364,7 +2373,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2378,7 +2387,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -2390,7 +2399,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2404,7 +2413,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -2416,7 +2425,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2430,7 +2439,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -2442,7 +2451,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2456,7 +2465,7 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -2468,7 +2477,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2482,7 +2491,7 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -2494,7 +2503,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2508,7 +2517,7 @@
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -2520,7 +2529,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2534,7 +2543,7 @@
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -2546,7 +2555,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2560,7 +2569,7 @@
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -2572,7 +2581,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2586,7 +2595,7 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F12">
         <v>2</v>
@@ -2598,7 +2607,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2612,7 +2621,7 @@
         <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F13">
         <v>2</v>
@@ -2624,7 +2633,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2638,7 +2647,7 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F14">
         <v>2</v>
@@ -2650,7 +2659,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2664,7 +2673,7 @@
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F15">
         <v>2</v>
@@ -2676,7 +2685,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2690,7 +2699,7 @@
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F16">
         <v>2</v>
@@ -2702,7 +2711,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2716,7 +2725,7 @@
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F17">
         <v>2</v>
@@ -2728,7 +2737,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2742,7 +2751,7 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -2754,7 +2763,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2768,7 +2777,7 @@
         <v>2</v>
       </c>
       <c r="E19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F19">
         <v>2</v>

</xml_diff>

<commit_message>
Fix bug - unstable engine
</commit_message>
<xml_diff>
--- a/Timetable-template.xlsx
+++ b/Timetable-template.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duc.le/Desktop/school/unitime-do-an/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs\BK - HCMUT\Programs\Github\unitime-do-an\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F930D8D-0C5E-7744-A45C-A1E1C759B701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20240" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="765" windowWidth="34560" windowHeight="20235" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Subject" sheetId="1" r:id="rId1"/>
@@ -363,7 +362,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -717,21 +716,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.1640625" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="14.1640625" customWidth="1"/>
+    <col min="2" max="2" width="14.125" customWidth="1"/>
+    <col min="4" max="4" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -745,7 +744,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -759,7 +758,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -773,7 +772,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -787,7 +786,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -801,7 +800,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -815,7 +814,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -829,7 +828,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -843,7 +842,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -864,21 +863,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.1640625" customWidth="1"/>
+    <col min="4" max="4" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.125" customWidth="1"/>
     <col min="8" max="9" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -898,7 +897,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -915,7 +914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -932,7 +931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -949,7 +948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -969,7 +968,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -989,7 +988,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1009,7 +1008,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1026,7 +1025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1046,7 +1045,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1063,7 +1062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1083,7 +1082,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1109,19 +1108,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1132,7 +1131,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1143,7 +1142,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1154,7 +1153,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1165,7 +1164,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1176,7 +1175,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1187,7 +1186,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1198,7 +1197,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1209,7 +1208,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1220,7 +1219,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1237,19 +1236,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1260,7 +1259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1271,7 +1270,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1282,7 +1281,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1293,7 +1292,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1304,7 +1303,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1315,7 +1314,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1326,7 +1325,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1337,7 +1336,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1348,7 +1347,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1359,7 +1358,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1370,7 +1369,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1381,7 +1380,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1392,7 +1391,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1403,7 +1402,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1414,7 +1413,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1431,21 +1430,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1459,7 +1458,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1473,7 +1472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1487,7 +1486,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1501,7 +1500,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1515,7 +1514,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1529,7 +1528,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1543,7 +1542,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1557,7 +1556,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1571,7 +1570,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1585,7 +1584,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1599,7 +1598,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1613,7 +1612,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1627,7 +1626,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1641,7 +1640,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1655,7 +1654,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1669,7 +1668,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1683,7 +1682,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1697,7 +1696,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1711,7 +1710,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1725,7 +1724,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1739,7 +1738,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1753,7 +1752,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1767,7 +1766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1781,7 +1780,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1795,7 +1794,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1809,7 +1808,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1823,7 +1822,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1837,7 +1836,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1851,7 +1850,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1865,7 +1864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1879,7 +1878,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1893,7 +1892,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1907,7 +1906,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1921,7 +1920,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1935,7 +1934,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1949,7 +1948,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1963,7 +1962,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1977,7 +1976,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1991,7 +1990,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2005,7 +2004,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2019,7 +2018,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2033,7 +2032,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2047,7 +2046,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2061,7 +2060,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2075,7 +2074,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2089,7 +2088,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2103,7 +2102,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2117,7 +2116,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2131,7 +2130,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2145,7 +2144,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2159,7 +2158,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2173,7 +2172,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2184,7 +2183,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2195,7 +2194,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2206,7 +2205,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2217,7 +2216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2228,7 +2227,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2239,7 +2238,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2250,7 +2249,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2261,7 +2260,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2278,23 +2277,23 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2320,7 +2319,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2347,7 +2346,7 @@
       </c>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2374,7 +2373,7 @@
       </c>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2401,7 +2400,7 @@
       </c>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2428,7 +2427,7 @@
       </c>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2455,7 +2454,7 @@
       </c>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2482,7 +2481,7 @@
       </c>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2509,7 +2508,7 @@
       </c>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2536,7 +2535,7 @@
       </c>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2563,7 +2562,7 @@
       </c>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2590,7 +2589,7 @@
       </c>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2617,7 +2616,7 @@
       </c>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2644,7 +2643,7 @@
       </c>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2671,7 +2670,7 @@
       </c>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2698,7 +2697,7 @@
       </c>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2725,7 +2724,7 @@
       </c>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2752,7 +2751,7 @@
       </c>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2779,7 +2778,7 @@
       </c>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2811,27 +2810,27 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2866,7 +2865,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2891,12 +2890,8 @@
       <c r="H2">
         <v>1</v>
       </c>
-      <c r="J2" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2921,11 +2916,8 @@
       <c r="H3">
         <v>1</v>
       </c>
-      <c r="J3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2950,11 +2942,8 @@
       <c r="H4">
         <v>1</v>
       </c>
-      <c r="J4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2979,11 +2968,8 @@
       <c r="H5">
         <v>1</v>
       </c>
-      <c r="J5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3007,9 +2993,6 @@
       </c>
       <c r="H6">
         <v>1</v>
-      </c>
-      <c r="J6" t="b">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3019,21 +3002,21 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -3047,7 +3030,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3061,7 +3044,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3075,7 +3058,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3089,7 +3072,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3103,7 +3086,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3117,7 +3100,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3131,7 +3114,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3145,7 +3128,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3159,7 +3142,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3174,7 +3157,7 @@
       </c>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3188,7 +3171,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3202,7 +3185,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3216,7 +3199,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3230,7 +3213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3244,7 +3227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3258,7 +3241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3272,7 +3255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
fix minor scaleup bug
</commit_message>
<xml_diff>
--- a/Timetable-template.xlsx
+++ b/Timetable-template.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="102">
   <si>
     <t>DEPARTMENT</t>
   </si>
@@ -275,15 +275,6 @@
     <t>PREFERED_PERIOD</t>
   </si>
   <si>
-    <t>2-6,7-12</t>
-  </si>
-  <si>
-    <t>3-6,7-12</t>
-  </si>
-  <si>
-    <t>2,3,4</t>
-  </si>
-  <si>
     <t>SCALEUP_CLASS</t>
   </si>
   <si>
@@ -351,9 +342,6 @@
   </si>
   <si>
     <t>UNRESTRICTED</t>
-  </si>
-  <si>
-    <t>2</t>
   </si>
   <si>
     <t>MIN_ENTRANTS</t>
@@ -401,11 +389,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -888,7 +875,7 @@
         <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1436,7 +1423,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
@@ -2836,10 +2823,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2866,10 +2853,10 @@
         <v>68</v>
       </c>
       <c r="D1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F1" t="s">
         <v>69</v>
@@ -2881,16 +2868,16 @@
         <v>76</v>
       </c>
       <c r="I1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J1" t="s">
+        <v>97</v>
+      </c>
+      <c r="K1" t="s">
         <v>99</v>
       </c>
-      <c r="J1" t="s">
-        <v>100</v>
-      </c>
-      <c r="K1" t="s">
-        <v>102</v>
-      </c>
       <c r="L1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -2898,172 +2885,24 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F2">
-        <v>3</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="H2" t="s">
-        <v>77</v>
+        <v>2</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
-      <c r="G3" t="s">
-        <v>79</v>
-      </c>
-      <c r="H3" t="s">
-        <v>77</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-      <c r="G4" t="s">
-        <v>79</v>
-      </c>
-      <c r="H4" t="s">
-        <v>78</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-      <c r="G5" t="s">
-        <v>79</v>
-      </c>
-      <c r="H5" t="s">
-        <v>77</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6">
-        <v>2</v>
-      </c>
-      <c r="G6" t="s">
-        <v>79</v>
-      </c>
-      <c r="H6" t="s">
-        <v>77</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-      <c r="F7">
-        <v>2</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="L7" t="b">
+      <c r="L2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3107,10 +2946,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D2">
         <v>10</v>
@@ -3121,10 +2960,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D3">
         <v>10</v>
@@ -3135,10 +2974,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D4">
         <v>10</v>
@@ -3149,10 +2988,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D5">
         <v>10</v>
@@ -3163,10 +3002,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D6">
         <v>10</v>
@@ -3177,10 +3016,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D7">
         <v>10</v>
@@ -3191,10 +3030,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D8">
         <v>10</v>
@@ -3205,10 +3044,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D9">
         <v>10</v>
@@ -3219,10 +3058,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D10">
         <v>10</v>
@@ -3234,10 +3073,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D11">
         <v>10</v>
@@ -3248,10 +3087,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D12">
         <v>10</v>
@@ -3262,10 +3101,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D13">
         <v>10</v>
@@ -3276,10 +3115,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -3290,10 +3129,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -3304,10 +3143,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -3318,10 +3157,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -3332,10 +3171,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D18">
         <v>0</v>

</xml_diff>